<commit_message>
ajout videos et images
</commit_message>
<xml_diff>
--- a/rapport/rapport_ihm.xlsx
+++ b/rapport/rapport_ihm.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.7976718296779319</v>
+        <v>1.835123164180666</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.7976718296779319</v>
+        <v>1.835123164180666</v>
       </c>
     </row>
     <row r="3">
@@ -488,10 +488,49 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7976718296779319</v>
+        <v>0.9234578654525802</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.amazon.fr/deals?ref_=nav_cs_gb</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>66</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.278420568435639</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.amazon.fr/deal/3a51f27b?showVariations=true&amp;pf_rd_r=JTA1B547JDKMBK143S96&amp;pf_rd_t=Events&amp;pf_rd_i=deals&amp;pf_rd_p=3c3f3ff2-f80e-428b-aff0-b0531c852487&amp;pf_rd_s=slot-14&amp;ref=dlx_deals_gd_dcl_img_1_3a51f27b_dt_sl14_87</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>69</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.599036199888587</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.amazon.fr/gp/your-account/order-history?ref_=ya_d_c_yo</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>79</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.835123164180666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>